<commit_message>
possible PDT-C errors/inconsistencies reported to Maruska
</commit_message>
<xml_diff>
--- a/tecto2umr/pdt-c-functors-comments.xlsx
+++ b/tecto2umr/pdt-c-functors-comments.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lopatkova\SVN\GitHub-UMR\tecto2umr\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="24915" windowHeight="14130"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="24920" windowHeight="14130"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -1425,9 +1430,6 @@
     <t>NOT in UMR, NEW to cover this nuance</t>
   </si>
   <si>
-    <t>NOT in UMR, NEW to cover EFF</t>
-  </si>
-  <si>
     <t>NORM</t>
   </si>
   <si>
@@ -1692,13 +1694,17 @@
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">NOT in UMR, NEW to cover EFF
+TODO - nesedí pro slovesa komunikace! </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1943,8 +1949,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hypertextový odkaz" xfId="1" builtinId="8"/>
-    <cellStyle name="Normální" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1952,14 +1958,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv systému Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Kancelář">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1997,9 +2006,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kancelář">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2034,7 +2043,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2069,7 +2078,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kancelář">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2246,24 +2255,24 @@
   <dimension ref="A1:J122"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F93" sqref="F93"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="3.42578125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="4"/>
+    <col min="1" max="1" width="3.453125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="9.1796875" style="4"/>
     <col min="3" max="3" width="10" style="5" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="14.54296875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="15.54296875" style="6" customWidth="1"/>
     <col min="6" max="6" width="62" style="17" customWidth="1"/>
-    <col min="7" max="7" width="37.28515625" style="14" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" style="16" customWidth="1"/>
-    <col min="9" max="9" width="35.42578125" style="16" customWidth="1"/>
-    <col min="10" max="10" width="74.5703125" customWidth="1"/>
+    <col min="7" max="7" width="37.26953125" style="14" customWidth="1"/>
+    <col min="8" max="8" width="13.26953125" style="16" customWidth="1"/>
+    <col min="9" max="9" width="35.453125" style="16" customWidth="1"/>
+    <col min="10" max="10" width="74.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" s="6">
         <v>0</v>
       </c>
@@ -2295,7 +2304,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" s="6">
         <v>0</v>
       </c>
@@ -2306,10 +2315,10 @@
         <v>10207</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="6">
         <v>0</v>
       </c>
@@ -2320,10 +2329,10 @@
         <v>8427</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="6">
         <v>0</v>
       </c>
@@ -2334,10 +2343,10 @@
         <v>2793</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" s="6">
         <v>0</v>
       </c>
@@ -2348,11 +2357,11 @@
         <v>209767</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" s="6">
         <v>0</v>
       </c>
@@ -2363,24 +2372,24 @@
         <v>422</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" s="6">
         <v>0</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="116">
       <c r="A8" s="6">
         <v>1</v>
       </c>
@@ -2403,7 +2412,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="165" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="159.5">
       <c r="A9" s="6">
         <v>2</v>
       </c>
@@ -2426,7 +2435,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="29">
       <c r="A10" s="6">
         <v>3</v>
       </c>
@@ -2449,7 +2458,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="58">
       <c r="A11" s="6">
         <v>4</v>
       </c>
@@ -2478,7 +2487,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="29">
       <c r="A12" s="6">
         <v>5</v>
       </c>
@@ -2495,7 +2504,7 @@
         <v>107</v>
       </c>
       <c r="G12" s="19" t="s">
-        <v>175</v>
+        <v>199</v>
       </c>
       <c r="H12" s="16" t="s">
         <v>81</v>
@@ -2504,23 +2513,23 @@
         <v>98</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10">
       <c r="A13" s="6">
         <v>6</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E13" s="2"/>
       <c r="G13" s="19"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="A14" s="6">
         <v>7</v>
       </c>
@@ -2540,7 +2549,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="A15" s="6">
         <v>8</v>
       </c>
@@ -2554,11 +2563,11 @@
         <v>84</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="A16" s="6">
         <v>9</v>
       </c>
@@ -2578,7 +2587,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9">
       <c r="A17" s="6">
         <v>10</v>
       </c>
@@ -2592,14 +2601,14 @@
         <v>84</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F17" s="2"/>
       <c r="H17" s="16" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9">
       <c r="A18" s="6">
         <v>11</v>
       </c>
@@ -2613,11 +2622,11 @@
         <v>104</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9">
       <c r="A19" s="6">
         <v>12</v>
       </c>
@@ -2631,7 +2640,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9">
       <c r="A20" s="6">
         <v>13</v>
       </c>
@@ -2645,7 +2654,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9">
       <c r="A21" s="6">
         <v>14</v>
       </c>
@@ -2659,7 +2668,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9">
       <c r="A22" s="6">
         <v>15</v>
       </c>
@@ -2673,21 +2682,21 @@
         <v>83</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9">
       <c r="A23" s="6">
         <v>16</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="43.5">
       <c r="A24" s="6">
         <v>17</v>
       </c>
@@ -2704,10 +2713,10 @@
         <v>107</v>
       </c>
       <c r="F24" s="17" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G24" s="22" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H24" s="16" t="s">
         <v>85</v>
@@ -2716,7 +2725,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9">
       <c r="A25" s="6">
         <v>18</v>
       </c>
@@ -2730,7 +2739,7 @@
         <v>106</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F25" s="17" t="s">
         <v>111</v>
@@ -2742,7 +2751,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="43.5">
       <c r="A26" s="6">
         <v>19</v>
       </c>
@@ -2768,7 +2777,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9">
       <c r="A27" s="6">
         <v>20</v>
       </c>
@@ -2794,22 +2803,22 @@
         <v>97</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9">
       <c r="A28" s="6">
         <v>21</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9">
       <c r="A29" s="6">
         <v>22</v>
       </c>
@@ -2832,7 +2841,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="29">
       <c r="A30" s="6">
         <v>23</v>
       </c>
@@ -2855,7 +2864,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9">
       <c r="A31" s="6">
         <v>24</v>
       </c>
@@ -2869,10 +2878,10 @@
         <v>160</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
       <c r="A32" s="6">
         <v>25</v>
       </c>
@@ -2886,11 +2895,11 @@
         <v>157</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F32" s="2"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9">
       <c r="A33" s="6">
         <v>26</v>
       </c>
@@ -2910,22 +2919,22 @@
         <v>120</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9">
       <c r="A34" s="6">
         <v>27</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E34" s="2"/>
     </row>
-    <row r="35" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9">
       <c r="A35" s="6">
         <v>28</v>
       </c>
@@ -2936,7 +2945,7 @@
         <v>12042</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>107</v>
@@ -2948,7 +2957,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9">
       <c r="A36" s="6">
         <v>29</v>
       </c>
@@ -2968,7 +2977,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9">
       <c r="A37" s="6">
         <v>30</v>
       </c>
@@ -2982,13 +2991,13 @@
         <v>172</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G37" s="19" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9">
       <c r="A38" s="6">
         <v>31</v>
       </c>
@@ -3008,7 +3017,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9">
       <c r="A39" s="6">
         <v>32</v>
       </c>
@@ -3031,7 +3040,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9">
       <c r="A40" s="6">
         <v>33</v>
       </c>
@@ -3054,7 +3063,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" ht="29">
       <c r="A41" s="6">
         <v>34</v>
       </c>
@@ -3077,12 +3086,12 @@
         <v>93</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9">
       <c r="A42" s="6">
         <v>35</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C42" s="8">
         <v>0</v>
@@ -3091,13 +3100,13 @@
         <v>172</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G42" s="19" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9">
       <c r="A43" s="6">
         <v>36</v>
       </c>
@@ -3117,7 +3126,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9">
       <c r="A44" s="6">
         <v>37</v>
       </c>
@@ -3128,16 +3137,16 @@
         <v>1617</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G44" s="19" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9">
       <c r="A45" s="6">
         <v>38</v>
       </c>
@@ -3151,25 +3160,25 @@
         <v>162</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
       <c r="A46" s="6">
         <v>39</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E46" s="2"/>
     </row>
-    <row r="47" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" ht="29">
       <c r="A47" s="6">
         <v>40</v>
       </c>
@@ -3195,7 +3204,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9">
       <c r="A48" s="6">
         <v>41</v>
       </c>
@@ -3206,13 +3215,13 @@
         <v>656</v>
       </c>
       <c r="D48" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="E48" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="E48" s="6" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:9" ht="43.5">
       <c r="A49" s="6">
         <v>42</v>
       </c>
@@ -3229,13 +3238,13 @@
         <v>107</v>
       </c>
       <c r="F49" s="17" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G49" s="22" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
       <c r="A50" s="6">
         <v>43</v>
       </c>
@@ -3249,26 +3258,26 @@
         <v>159</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F50" s="2"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9">
       <c r="A51" s="6">
         <v>44</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F51" s="2"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9">
       <c r="A52" s="6">
         <v>45</v>
       </c>
@@ -3286,23 +3295,23 @@
         <v>75</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9">
       <c r="A53" s="6">
         <v>46</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E53" s="2"/>
       <c r="G53" s="21"/>
     </row>
-    <row r="54" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" ht="43.5">
       <c r="A54" s="6">
         <v>47</v>
       </c>
@@ -3316,10 +3325,10 @@
         <v>130</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G54" s="22" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H54" s="16" t="s">
         <v>94</v>
@@ -3328,7 +3337,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9">
       <c r="A55" s="6">
         <v>48</v>
       </c>
@@ -3345,10 +3354,10 @@
         <v>107</v>
       </c>
       <c r="F55" s="17" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9">
       <c r="A56" s="6">
         <v>49</v>
       </c>
@@ -3362,10 +3371,10 @@
         <v>77</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="29">
       <c r="A57" s="6">
         <v>50</v>
       </c>
@@ -3379,13 +3388,13 @@
         <v>67</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G57" s="23" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9">
       <c r="A58" s="6">
         <v>51</v>
       </c>
@@ -3399,29 +3408,29 @@
         <v>67</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F58" s="2"/>
       <c r="H58" s="16" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9">
       <c r="A59" s="6">
         <v>52</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D59" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F59" s="2"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9">
       <c r="A60" s="6">
         <v>53</v>
       </c>
@@ -3438,7 +3447,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9">
       <c r="A61" s="6">
         <v>54</v>
       </c>
@@ -3456,7 +3465,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9">
       <c r="A62" s="6">
         <v>55</v>
       </c>
@@ -3474,23 +3483,23 @@
         <v>75</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9">
       <c r="A63" s="6">
         <v>56</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D63" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E63" s="2"/>
       <c r="G63" s="21"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9">
       <c r="A64" s="6">
         <v>57</v>
       </c>
@@ -3501,13 +3510,13 @@
         <v>7134</v>
       </c>
       <c r="D64" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="E64" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="E64" s="2" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:7">
       <c r="A65" s="6">
         <v>58</v>
       </c>
@@ -3518,13 +3527,13 @@
         <v>99</v>
       </c>
       <c r="D65" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="E65" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="E65" s="6" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="1:7">
       <c r="A66" s="6">
         <v>59</v>
       </c>
@@ -3538,10 +3547,10 @@
         <v>69</v>
       </c>
       <c r="E66" s="6" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
       <c r="A67" s="6">
         <v>60</v>
       </c>
@@ -3552,16 +3561,16 @@
         <v>211</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E67" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G67" s="19" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7">
       <c r="A68" s="6">
         <v>66</v>
       </c>
@@ -3572,13 +3581,13 @@
         <v>3054</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E68" s="6" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
       <c r="A69" s="6">
         <v>67</v>
       </c>
@@ -3589,16 +3598,16 @@
         <v>4122</v>
       </c>
       <c r="D69" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="E69" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="G69" s="19" t="s">
         <v>193</v>
       </c>
-      <c r="E69" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="G69" s="19" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="1:7">
       <c r="A70" s="6">
         <v>68</v>
       </c>
@@ -3612,10 +3621,10 @@
         <v>69</v>
       </c>
       <c r="E70" s="6" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
       <c r="A71" s="6">
         <v>69</v>
       </c>
@@ -3626,28 +3635,28 @@
         <v>491</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
       <c r="A72" s="6">
         <v>70</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C72" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D72" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E72" s="2"/>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7">
       <c r="A73" s="6">
         <v>71</v>
       </c>
@@ -3665,23 +3674,23 @@
         <v>75</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7">
       <c r="A74" s="6">
         <v>72</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C74" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D74" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E74" s="2"/>
       <c r="G74" s="21"/>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7">
       <c r="A75" s="6">
         <v>73</v>
       </c>
@@ -3697,23 +3706,23 @@
         <v>75</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7">
       <c r="A76" s="6">
         <v>74</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C76" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D76" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E76" s="2"/>
       <c r="G76" s="27"/>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7">
       <c r="A77" s="6">
         <v>75</v>
       </c>
@@ -3729,23 +3738,23 @@
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7">
       <c r="A78" s="6">
         <v>76</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C78" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D78" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E78" s="2"/>
       <c r="G78" s="28"/>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7">
       <c r="A79" s="6">
         <v>77</v>
       </c>
@@ -3761,7 +3770,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7">
       <c r="A80" s="6">
         <v>78</v>
       </c>
@@ -3777,7 +3786,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7">
       <c r="A81" s="6">
         <v>79</v>
       </c>
@@ -3793,7 +3802,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7">
       <c r="A82" s="6">
         <v>80</v>
       </c>
@@ -3809,7 +3818,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7">
       <c r="A83" s="6">
         <v>81</v>
       </c>
@@ -3825,21 +3834,21 @@
         <v>75</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7">
       <c r="A84" s="6">
         <v>82</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C84" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D84" s="7" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7">
       <c r="D86" s="10" t="s">
         <v>119</v>
       </c>
@@ -3847,100 +3856,100 @@
         <v>107</v>
       </c>
       <c r="F86" s="17" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7">
       <c r="D88" s="4" t="s">
         <v>126</v>
       </c>
       <c r="E88" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F88" s="2"/>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7">
       <c r="D89" s="4" t="s">
         <v>127</v>
       </c>
       <c r="E89" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F89" s="2"/>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7">
       <c r="D90" s="4" t="s">
         <v>128</v>
       </c>
       <c r="E90" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F90" s="2"/>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7">
       <c r="D91" s="4" t="s">
         <v>129</v>
       </c>
       <c r="E91" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F91" s="2"/>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7">
       <c r="D92" s="4" t="s">
         <v>132</v>
       </c>
       <c r="E92" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F92" s="2"/>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7">
       <c r="D93" s="4" t="s">
         <v>133</v>
       </c>
       <c r="E93" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F93" s="2"/>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7">
       <c r="D94" s="4" t="s">
         <v>134</v>
       </c>
       <c r="E94" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F94" s="2"/>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7">
       <c r="D95" s="4" t="s">
         <v>135</v>
       </c>
       <c r="E95" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F95" s="2"/>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7">
       <c r="D96" s="4" t="s">
         <v>136</v>
       </c>
       <c r="E96" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F96" s="2"/>
     </row>
-    <row r="97" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="4:6">
       <c r="D97" s="4" t="s">
         <v>137</v>
       </c>
       <c r="E97" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F97" s="2"/>
     </row>
-    <row r="99" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="4:6">
       <c r="D99" s="4" t="s">
         <v>138</v>
       </c>
@@ -3948,7 +3957,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="100" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="4:6">
       <c r="D100" s="4" t="s">
         <v>139</v>
       </c>
@@ -3956,7 +3965,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="101" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="4:6">
       <c r="D101" s="4" t="s">
         <v>140</v>
       </c>
@@ -3964,7 +3973,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="102" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="4:6">
       <c r="D102" s="4" t="s">
         <v>96</v>
       </c>
@@ -3972,7 +3981,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="103" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="4:6">
       <c r="D103" s="4" t="s">
         <v>141</v>
       </c>
@@ -3980,7 +3989,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="105" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="4:6">
       <c r="D105" s="11" t="s">
         <v>82</v>
       </c>
@@ -3991,10 +4000,10 @@
         <v>142</v>
       </c>
     </row>
-    <row r="106" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="4:6">
       <c r="E106" s="20"/>
     </row>
-    <row r="107" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="4:6">
       <c r="D107" s="11" t="s">
         <v>143</v>
       </c>
@@ -4005,7 +4014,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="108" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="4:6">
       <c r="D108" s="11" t="s">
         <v>144</v>
       </c>
@@ -4016,7 +4025,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="109" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="4:6">
       <c r="D109" s="11" t="s">
         <v>145</v>
       </c>
@@ -4027,7 +4036,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="110" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="4:6">
       <c r="D110" s="12" t="s">
         <v>146</v>
       </c>
@@ -4038,7 +4047,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="111" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="4:6">
       <c r="D111" s="12" t="s">
         <v>147</v>
       </c>
@@ -4049,7 +4058,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="112" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="4:6">
       <c r="D112" s="11" t="s">
         <v>148</v>
       </c>
@@ -4060,7 +4069,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="113" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="4:6">
       <c r="D113" s="11" t="s">
         <v>149</v>
       </c>
@@ -4071,12 +4080,12 @@
         <v>155</v>
       </c>
     </row>
-    <row r="114" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="4:6">
       <c r="D114" s="11"/>
       <c r="E114" s="3"/>
       <c r="F114" s="2"/>
     </row>
-    <row r="115" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="4:6">
       <c r="D115" s="3" t="s">
         <v>164</v>
       </c>
@@ -4087,7 +4096,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="116" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="4:6">
       <c r="D116" s="3" t="s">
         <v>165</v>
       </c>
@@ -4098,7 +4107,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="117" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="4:6">
       <c r="D117" s="3" t="s">
         <v>166</v>
       </c>
@@ -4109,11 +4118,11 @@
         <v>167</v>
       </c>
     </row>
-    <row r="118" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="4:6">
       <c r="D118" s="3"/>
       <c r="E118" s="20"/>
     </row>
-    <row r="119" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="4:6">
       <c r="D119" s="6" t="s">
         <v>156</v>
       </c>
@@ -4124,7 +4133,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="120" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="4:6">
       <c r="D120" s="6" t="s">
         <v>158</v>
       </c>
@@ -4135,7 +4144,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="121" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="4:6">
       <c r="D121" s="6" t="s">
         <v>161</v>
       </c>
@@ -4146,7 +4155,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="122" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="4:6">
       <c r="D122" s="6"/>
       <c r="F122" s="2"/>
     </row>
@@ -4169,7 +4178,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4181,7 +4190,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>